<commit_message>
camios casos de uso
</commit_message>
<xml_diff>
--- a/doc/casos_De_Uso.xlsx
+++ b/doc/casos_De_Uso.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianacastro/Desktop/LibreriaVirtualCrackTheCode/LibreriaVirtualCrackTheCode/doc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5A3135-48CD-0046-A6AE-D57A383572C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1920" yWindow="-27960" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>Requerimientos de Acción</t>
   </si>
@@ -188,37 +197,42 @@
   </si>
   <si>
     <t>Visualizar los ultimos 4 digitos del numero de tarjeta</t>
+  </si>
+  <si>
+    <t>di</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -228,7 +242,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -298,68 +312,53 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -549,26 +548,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="61.88"/>
-    <col customWidth="1" min="2" max="2" width="54.13"/>
-    <col customWidth="1" min="6" max="6" width="38.25"/>
-    <col customWidth="1" min="7" max="7" width="16.0"/>
+    <col min="1" max="1" width="61.83203125" customWidth="1"/>
+    <col min="2" max="2" width="54.1640625" customWidth="1"/>
+    <col min="6" max="6" width="38.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -602,7 +606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -619,7 +623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -633,7 +637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -647,7 +651,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
@@ -661,7 +665,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -675,7 +679,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
@@ -689,7 +693,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -703,7 +707,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>35</v>
       </c>
@@ -717,7 +721,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
@@ -731,7 +735,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
         <v>43</v>
       </c>
@@ -745,7 +749,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
@@ -753,7 +757,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
@@ -761,7 +765,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
         <v>50</v>
       </c>
@@ -769,7 +773,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
         <v>52</v>
       </c>
@@ -777,30 +781,33 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18">
+      <c r="F17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios a los casos de uso
</commit_message>
<xml_diff>
--- a/doc/casos_De_Uso.xlsx
+++ b/doc/casos_De_Uso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dianacastro/Desktop/LibreriaVirtualCrackTheCode/LibreriaVirtualCrackTheCode/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5A3135-48CD-0046-A6AE-D57A383572C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0398D2-3E56-914B-B667-CD2AD99A305F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="-27960" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4660" yWindow="-27960" windowWidth="26060" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Requerimientos de Acción</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Comprador</t>
   </si>
   <si>
-    <t>Iniciar sesión y cerrar sesión usuario cliente</t>
-  </si>
-  <si>
     <t>Juan</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>Visualizar el genero del autor</t>
   </si>
   <si>
-    <t>Iniciar sesión y cerrar sesión usuario admin</t>
-  </si>
-  <si>
     <t>RF-15 Agregar libros al carrito de compras</t>
   </si>
   <si>
@@ -199,14 +193,23 @@
     <t>Visualizar los ultimos 4 digitos del numero de tarjeta</t>
   </si>
   <si>
-    <t>di</t>
+    <t>Cerrar sesión usuario admin</t>
+  </si>
+  <si>
+    <t>Iniciar sesión usuario admin</t>
+  </si>
+  <si>
+    <t>Cerrar sesión usuario cliente</t>
+  </si>
+  <si>
+    <t>Iniciar sesión usuario cliente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -236,8 +239,15 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +317,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD0E0E3"/>
+        <bgColor rgb="FFD0E0E3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor rgb="FFD0E0E3"/>
       </patternFill>
     </fill>
@@ -323,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -340,6 +356,8 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,10 +576,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -589,222 +607,236 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="6" t="s">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="F2" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>59</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="F6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="G6" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="F8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="G8" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="13" t="s">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="5" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="5" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="5" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>